<commit_message>
(CENSORED data)  Added wy2016-17 Combined Outflow wwMeHg  folder;  Updated wwMeHg model results file for wy2016-17.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwMeHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwMeHg Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{641363C0-9BF4-4299-93B2-C1750A8DDA2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EDC45FCF-114D-472A-B00E-F519DA0248BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,12 +81,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{C6717B38-828E-4701-8FB0-3099A8E3DB6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rose, Shanna Lynn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There were 5 censored values for this parameter, 29 uncensored.
+Used 0.05 ng/L (one-half of the MDL) in calculations for the constituent censored data in the text file.
+-12/3/18</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="815">
   <si>
     <t>Model #</t>
   </si>
@@ -2012,6 +2038,525 @@
   </si>
   <si>
     <t>Number of Uncensored Observations: 29; Period of record: 2016-01-20 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm1 &lt;- loadReg(wwMeHg ~model(1), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 34</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0699</t>
+  </si>
+  <si>
+    <t>(Intercept)   -6.737     0.1050  -64.19       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.170     0.0631   18.54       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3668</t>
+  </si>
+  <si>
+    <t>R-squared: 91.49 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 83.75 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.874</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.29</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.02 0.02</t>
+  </si>
+  <si>
+    <t>Obs   0   0   0 0.01 0.02 0.03 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -4.608 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8075</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm2 &lt;- loadReg(wwMeHg ~model(2), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Estimate Std. Error  z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -6.764271    0.16708 -40.4854  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.170044    0.06407  18.2634  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.009802    0.04652   0.2107  0.8254</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3781</t>
+  </si>
+  <si>
+    <t>R-squared: 91.5 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 83.8 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.8434</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.289</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.02 0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -3.378 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8141</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm3 &lt;- loadReg(wwMeHg ~model(3), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept) -6.73888    0.10645 -63.3043  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.15843    0.07039  16.4579  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      0.09765    0.24725   0.3949  0.6795</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3767</t>
+  </si>
+  <si>
+    <t>R-squared: 91.53 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 83.93 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.9149</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2746</t>
+  </si>
+  <si>
+    <t>lnQ     1.211</t>
+  </si>
+  <si>
+    <t>DECTIME 1.211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -3.498 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8121</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm4 &lt;- loadReg(wwMeHg ~model(4), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -5.9324    0.64923  -9.138  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2061    0.06957  17.335  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.7932    0.56280  -1.409  0.1398</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.5742    0.55190  -1.040  0.2723</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3657</t>
+  </si>
+  <si>
+    <t>R-squared: 92.04 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 86.05 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7719</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.263</t>
+  </si>
+  <si>
+    <t>lnQ         1.219</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.817</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.874</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -1.616 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.868</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm5 &lt;- loadReg(wwMeHg ~model(5), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Estimate Std. Error   z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -6.749966    0.17471 -38.63418  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.159300    0.07235  16.02395  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.004055    0.05017   0.08082  0.9314</t>
+  </si>
+  <si>
+    <t>DECTIME      0.090337    0.26710   0.33821  0.7191</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3892</t>
+  </si>
+  <si>
+    <t>G-squared: 83.93 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.9095</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2756</t>
+  </si>
+  <si>
+    <t>lnQ     1.239</t>
+  </si>
+  <si>
+    <t>lnQ2    1.130</t>
+  </si>
+  <si>
+    <t>DECTIME 1.368</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -3.013 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8142</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm6 &lt;- loadReg(wwMeHg ~model(6), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.86152    0.69925 -8.3825  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.20705    0.07072 17.0672  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.01618    0.05317 -0.3042  0.7420</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.84214    0.59374 -1.4184  0.1310</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.57330    0.56045 -1.0229  0.2723</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3771</t>
+  </si>
+  <si>
+    <t>R-squared: 92.07 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 86.16 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7807</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2528</t>
+  </si>
+  <si>
+    <t>lnQ         1.222</t>
+  </si>
+  <si>
+    <t>lnQ2        1.309</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -3.24 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8637</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm7 &lt;- loadReg(wwMeHg ~model(7), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -5.5246    0.84594 -6.5307  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2542    0.09441 13.2839  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.2516    0.33109 -0.7598  0.4130</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.1795    0.76147 -1.5490  0.1002</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.8714    0.67971 -1.2820  0.1710</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.371</t>
+  </si>
+  <si>
+    <t>R-squared: 92.2 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 86.72 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.4542</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2869</t>
+  </si>
+  <si>
+    <t>lnQ         2.213</t>
+  </si>
+  <si>
+    <t>DECTIME     2.206</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.888</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.793</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -2.132 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8782</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm8 &lt;- loadReg(wwMeHg ~model(8), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.50622    0.86941 -6.3333  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.25260    0.09661 12.9651  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.00815    0.05486 -0.1486  0.8700</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.24086    0.34444 -0.6993  0.4429</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.18776    0.77662 -1.5294  0.0986</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.85834    0.69706 -1.2314  0.1806</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3839</t>
+  </si>
+  <si>
+    <t>G-squared: 86.75 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.4904</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2816</t>
+  </si>
+  <si>
+    <t>lnQ         2.240</t>
+  </si>
+  <si>
+    <t>lnQ2        1.369</t>
+  </si>
+  <si>
+    <t>DECTIME     2.307</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.924</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.887</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -2.898 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8757</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm9 &lt;- loadReg(wwMeHg ~model(9), data = wwMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwMeHg_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.47020    0.88424 -6.1863  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.28866    0.12164 10.5938  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.01444    0.05701 -0.2533  0.7763</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.33871    0.40029 -0.8462  0.3455</t>
+  </si>
+  <si>
+    <t>DECTIME2     0.92727    1.85527  0.4998  0.5758</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.45043    0.94654 -1.5323  0.0922</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.98592    0.75128 -1.3123  0.1471</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3945</t>
+  </si>
+  <si>
+    <t>R-squared: 92.27 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 87.06 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.591</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2808</t>
+  </si>
+  <si>
+    <t>lnQ          3.456</t>
+  </si>
+  <si>
+    <t>lnQ2         1.440</t>
+  </si>
+  <si>
+    <t>DECTIME      3.033</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.943</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 10.009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  6.656</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -2.085 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8815</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34; Period of record: 2016-01-20 to 2017-04-26</t>
   </si>
 </sst>
 </file>
@@ -2271,7 +2816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2375,6 +2920,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2387,47 +2971,14 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2435,186 +2986,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3147,7 +3518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3161,10 +3532,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>20</v>
@@ -3203,24 +3574,24 @@
       <c r="L2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="49"/>
       <c r="Z4" s="18" t="s">
         <v>50</v>
       </c>
@@ -3235,21 +3606,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="47" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="47"/>
+      <c r="L5" s="40"/>
       <c r="Z5" s="18" t="s">
         <v>51</v>
       </c>
@@ -3747,36 +4118,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="44" t="s">
         <v>457</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="47" t="s">
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="47"/>
+      <c r="L18" s="40"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -4257,36 +4628,36 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="49"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="44" t="s">
         <v>641</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="47" t="s">
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="47"/>
+      <c r="L31" s="40"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -4387,7 +4758,7 @@
       <c r="B34" s="11">
         <v>0</v>
       </c>
-      <c r="C34" s="52">
+      <c r="C34" s="39">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="D34" s="34" t="s">
@@ -4734,7 +5105,7 @@
       <c r="E41" s="6">
         <v>0.82709999999999995</v>
       </c>
-      <c r="F41" s="51">
+      <c r="F41" s="38">
         <v>0.20130000000000001</v>
       </c>
       <c r="G41" s="6">
@@ -4767,22 +5138,24 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="43"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="49"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B44" s="44"/>
+      <c r="B44" s="44" t="s">
+        <v>814</v>
+      </c>
       <c r="C44" s="45"/>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -4791,10 +5164,10 @@
       <c r="H44" s="45"/>
       <c r="I44" s="45"/>
       <c r="J44" s="46"/>
-      <c r="K44" s="47" t="s">
+      <c r="K44" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="47"/>
+      <c r="L44" s="40"/>
     </row>
     <row r="45" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -4841,35 +5214,45 @@
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A46" s="27">
+      <c r="A46" s="11">
         <v>1</v>
       </c>
       <c r="B46" s="11">
         <v>0</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="34" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
+      <c r="I46" s="11">
+        <v>91.49</v>
+      </c>
+      <c r="J46" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K46" s="11">
+        <v>-4.6079999999999997</v>
+      </c>
+      <c r="L46" s="37">
+        <v>0.8075</v>
+      </c>
+      <c r="M46" s="11" t="s">
+        <v>276</v>
+      </c>
       <c r="N46" s="8" t="s">
         <v>16</v>
       </c>
@@ -4884,10 +5267,12 @@
       <c r="A47" s="27">
         <v>2</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="6">
         <v>0</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="25">
+        <v>0.82540000000000002</v>
+      </c>
       <c r="D47" s="10" t="s">
         <v>15</v>
       </c>
@@ -4900,13 +5285,21 @@
       <c r="G47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
+      <c r="I47" s="37">
+        <v>91.5</v>
+      </c>
+      <c r="J47" s="37">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="K47" s="37">
+        <v>-3.3780000000000001</v>
+      </c>
+      <c r="L47" s="37">
+        <v>0.81410000000000005</v>
+      </c>
       <c r="M47" s="27"/>
       <c r="N47" s="8" t="s">
         <v>16</v>
@@ -4922,13 +5315,15 @@
       <c r="A48" s="27">
         <v>3</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="6">
         <v>0</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="23"/>
+      <c r="D48" s="23">
+        <v>0.67949999999999999</v>
+      </c>
       <c r="E48" s="10" t="s">
         <v>15</v>
       </c>
@@ -4938,13 +5333,21 @@
       <c r="G48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
+      <c r="I48" s="37">
+        <v>91.53</v>
+      </c>
+      <c r="J48" s="37">
+        <v>0.27460000000000001</v>
+      </c>
+      <c r="K48" s="37">
+        <v>-3.4980000000000002</v>
+      </c>
+      <c r="L48" s="37">
+        <v>0.81210000000000004</v>
+      </c>
       <c r="M48" s="27"/>
       <c r="N48" s="8" t="s">
         <v>16</v>
@@ -4960,7 +5363,7 @@
       <c r="A49" s="27">
         <v>4</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -4972,15 +5375,27 @@
       <c r="E49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="11" t="s">
+      <c r="F49" s="6">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="G49" s="37">
+        <v>0.27229999999999999</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
+      <c r="I49" s="37">
+        <v>92.04</v>
+      </c>
+      <c r="J49" s="37">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="K49" s="37">
+        <v>-1.6160000000000001</v>
+      </c>
+      <c r="L49" s="37">
+        <v>0.86799999999999999</v>
+      </c>
       <c r="M49" s="27"/>
       <c r="N49" s="8" t="s">
         <v>16</v>
@@ -4996,11 +5411,15 @@
       <c r="A50" s="27">
         <v>5</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="6">
         <v>0</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="37">
+        <v>0.93140000000000001</v>
+      </c>
+      <c r="D50" s="37">
+        <v>0.71909999999999996</v>
+      </c>
       <c r="E50" s="10" t="s">
         <v>15</v>
       </c>
@@ -5010,13 +5429,21 @@
       <c r="G50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
+      <c r="I50" s="37">
+        <v>91.53</v>
+      </c>
+      <c r="J50" s="37">
+        <v>0.27560000000000001</v>
+      </c>
+      <c r="K50" s="37">
+        <v>-3.0129999999999999</v>
+      </c>
+      <c r="L50" s="37">
+        <v>0.81420000000000003</v>
+      </c>
       <c r="M50" s="27"/>
       <c r="N50" s="8" t="s">
         <v>16</v>
@@ -5032,25 +5459,39 @@
       <c r="A51" s="27">
         <v>6</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="6">
         <v>0</v>
       </c>
-      <c r="C51" s="27"/>
+      <c r="C51" s="37">
+        <v>0.74199999999999999</v>
+      </c>
       <c r="D51" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="11" t="s">
+      <c r="F51" s="6">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G51" s="37">
+        <v>0.27229999999999999</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
+      <c r="I51" s="37">
+        <v>92.07</v>
+      </c>
+      <c r="J51" s="37">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="K51" s="37">
+        <v>-3.24</v>
+      </c>
+      <c r="L51" s="37">
+        <v>0.86370000000000002</v>
+      </c>
       <c r="M51" s="27"/>
       <c r="N51" s="8" t="s">
         <v>16</v>
@@ -5066,25 +5507,39 @@
       <c r="A52" s="27">
         <v>7</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="6">
         <v>0</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6">
+        <v>0.41299999999999998</v>
+      </c>
       <c r="E52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="11" t="s">
+      <c r="F52" s="6">
+        <v>0.1002</v>
+      </c>
+      <c r="G52" s="37">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
+      <c r="I52" s="37">
+        <v>92.2</v>
+      </c>
+      <c r="J52" s="37">
+        <v>0.28689999999999999</v>
+      </c>
+      <c r="K52" s="37">
+        <v>-2.1320000000000001</v>
+      </c>
+      <c r="L52" s="37">
+        <v>0.87819999999999998</v>
+      </c>
       <c r="M52" s="27"/>
       <c r="N52" s="8" t="s">
         <v>16</v>
@@ -5100,23 +5555,39 @@
       <c r="A53" s="27">
         <v>8</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="6">
         <v>0</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="37">
+        <v>0.87</v>
+      </c>
+      <c r="D53" s="6">
+        <v>0.44290000000000002</v>
+      </c>
       <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="11" t="s">
+      <c r="F53" s="6">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="27"/>
+      <c r="I53" s="37">
+        <v>92.2</v>
+      </c>
+      <c r="J53" s="37">
+        <v>0.28160000000000002</v>
+      </c>
+      <c r="K53" s="37">
+        <v>-2.8980000000000001</v>
+      </c>
+      <c r="L53" s="37">
+        <v>0.87570000000000003</v>
+      </c>
       <c r="M53" s="27"/>
       <c r="N53" s="8" t="s">
         <v>16</v>
@@ -5132,21 +5603,39 @@
       <c r="A54" s="27">
         <v>9</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="6">
         <v>0</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="11" t="s">
+      <c r="C54" s="37">
+        <v>0.77629999999999999</v>
+      </c>
+      <c r="D54" s="6">
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0.57579999999999998</v>
+      </c>
+      <c r="F54" s="6">
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.14710000000000001</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
+      <c r="I54" s="37">
+        <v>92.27</v>
+      </c>
+      <c r="J54" s="37">
+        <v>0.28079999999999999</v>
+      </c>
+      <c r="K54" s="37">
+        <v>-2.085</v>
+      </c>
+      <c r="L54" s="37">
+        <v>0.88149999999999995</v>
+      </c>
       <c r="M54" s="27"/>
       <c r="N54" s="8" t="s">
         <v>16</v>
@@ -5164,34 +5653,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="42"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="47"/>
-      <c r="L57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="40"/>
+      <c r="L57" s="40"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="44"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="47" t="s">
+      <c r="B58" s="41"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="47"/>
+      <c r="L58" s="40"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -5431,6 +5920,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K58:L58"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B18:J18"/>
@@ -5443,85 +5938,79 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="K44:L44"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
-    <cfRule type="cellIs" dxfId="36" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="43" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="44" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="45" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55 K60:K1048576 K57 K29">
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="29" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="30" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="26" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46:L54 L33:L41 L20:L28">
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:K54 K33:K41 K20:K28">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54 C34 D35 C37:C38 D37 C40:C41 D39:D41 E41 F36:G36 F38:G40 C21 D22 C24:C25 D24 C27:C28 D26:D28 E28 F23:G23 F25:G28 G41">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L15">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K15">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8 D9 C11:C12 D11 C14:C15 D13:D15 E15 F10:G10 F12:G15">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12957,118 +13446,179 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FBE2AD-EC1E-4563-8289-C8C08DD23DD5}">
-  <dimension ref="A1:A528"/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A527"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="R17" sqref="R17:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -13077,1465 +13627,2277 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="16"/>
@@ -14544,10 +15906,9 @@
       <c r="A526" s="16"/>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A527" s="17"/>
-    </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A528" s="12"/>
+      <c r="A527" s="54" t="s">
+        <v>813</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>